<commit_message>
lesson16 - database - rdbms - 07.10.2022(2)
</commit_message>
<xml_diff>
--- a/1.RDBMS/JAVA15 - DangVanNhatMinh - Database Design.xlsx
+++ b/1.RDBMS/JAVA15 - DangVanNhatMinh - Database Design.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0E41900-4C0E-4A73-BA36-37EDE0D647FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9343F521-6382-4BAE-A423-833EB150D56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -551,7 +551,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -876,7 +876,9 @@
     <row r="15" spans="1:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>

</xml_diff>